<commit_message>
feat: add employee locality status and column management enhancements
- Add locality_status column to employee_core table and register in column_catalog
- Implement column renaming scripts for insurance and travel tables
- Add role-based column visibility controls and export options
- Enhance employee table with configurable column display
- Add schema validation tools and migration scripts
- Update employee forms with type-safe input handling
- Implement column visibility selection in directory view
</commit_message>
<xml_diff>
--- a/public/template_data.xlsx
+++ b/public/template_data.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\mti-employee\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scripts\Projects\mti-employee\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9672BB4F-6CA8-4225-BC97-F26F47DF00FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4CB472-C12C-42A3-8D0F-DD4040E321CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2636C959-2C22-4666-8DE2-CDBCA437C9A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{2636C959-2C22-4666-8DE2-CDBCA437C9A4}"/>
   </bookViews>
   <sheets>
     <sheet name="template_data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="65">
   <si>
     <t>insurance_endorsement</t>
   </si>
@@ -1077,9 +1091,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9308A9-C231-42AB-9418-F8C20B7F2C86}">
   <dimension ref="A1:BM1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="BJ1" workbookViewId="0">
+      <selection sqref="A1:BM1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="5.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1281,4 +1362,347 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F18C40-7574-4F17-8999-7C8E670A9D1A}">
+  <dimension ref="A1:A65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>